<commit_message>
Made the page load through Json now and JS
</commit_message>
<xml_diff>
--- a/ZorgTools.xlsx
+++ b/ZorgTools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\S5 Stage\InterActiveList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210EB901-7D9F-4604-B10B-2ABEDC35F94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8B7E26-83E1-4B7C-902C-A2D613171737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E00BBEE8-4644-4DCA-8691-B52A139901BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>E-health:Beeldbellen, ECD Electronisch clienten dossier</t>
   </si>
@@ -69,18 +69,6 @@
     <t>Wolk heupairbag valdetectie</t>
   </si>
   <si>
-    <t>ToolNaam</t>
-  </si>
-  <si>
-    <t>Tool Beschrijving</t>
-  </si>
-  <si>
-    <t>ToolImg</t>
-  </si>
-  <si>
-    <t>ToolLink</t>
-  </si>
-  <si>
     <t>We leven allemaal tegen woordig digitaal dus waarom niet bellen met je dokter. Of inzien hoe het met je gaat. Dat allemaal digitaal bij de hand.</t>
   </si>
   <si>
@@ -88,6 +76,36 @@
   </si>
   <si>
     <t>Null</t>
+  </si>
+  <si>
+    <t>Toolnaam</t>
+  </si>
+  <si>
+    <t>Toolbeschrijving</t>
+  </si>
+  <si>
+    <t>Toolimg</t>
+  </si>
+  <si>
+    <t>Toollink</t>
+  </si>
+  <si>
+    <t>Hoe werken IOT en Smart mobiles nou samen met de zorg? Vindt het hier uit</t>
+  </si>
+  <si>
+    <t>https://www.duurzaammbo.nl/images/foto2/domotica.jpg</t>
+  </si>
+  <si>
+    <t>Bedsensoren. Tenslotte willen we niet dat onze patienten een onrustigge nacht hebben. Hoe houden we dat in de gaten?</t>
+  </si>
+  <si>
+    <t>https://www.fundis.nl/wp-content/uploads/2019/05/FundiQare_Momo-Medical_Plaat-en-Box.jpg</t>
+  </si>
+  <si>
+    <t>Persoon kwijt of iemand met dementie. Maak gebruik van de Persoon alarm. Vaak gepaard met gps.</t>
+  </si>
+  <si>
+    <t>https://www.curamare.nl/images/content/page341/3ded8d9da1curamare-persoonsalarmering.jpg</t>
   </si>
 </sst>
 </file>
@@ -453,7 +471,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,16 +485,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -484,29 +502,56 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -549,8 +594,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{2E623B92-F184-4918-A35F-B63234A80043}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{B46671C8-63A3-49B5-B4EF-1CACFB8A9760}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{299DFFAB-1472-4D97-BB8D-603913F8C715}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{EF88D0AD-6763-4C9E-A952-C649B59621B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started working on the modals and encountered issues
</commit_message>
<xml_diff>
--- a/ZorgTools.xlsx
+++ b/ZorgTools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\S5 Stage\InterActiveList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8B7E26-83E1-4B7C-902C-A2D613171737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75887A7E-1246-4F68-8780-992BCB83BF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E00BBEE8-4644-4DCA-8691-B52A139901BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>E-health:Beeldbellen, ECD Electronisch clienten dossier</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>https://www.curamare.nl/images/content/page341/3ded8d9da1curamare-persoonsalarmering.jpg</t>
+  </si>
+  <si>
+    <t>https://www.google.nl/</t>
+  </si>
+  <si>
+    <t>https://Google.nl/,https://stackoverflow.com/questions/179713/how-to-change-the-href-attribute-for-a-hyperlink-using-jquery</t>
   </si>
 </sst>
 </file>
@@ -471,7 +477,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,8 +513,8 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -521,8 +527,8 @@
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -557,35 +563,56 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
@@ -597,8 +624,10 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{B46671C8-63A3-49B5-B4EF-1CACFB8A9760}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{299DFFAB-1472-4D97-BB8D-603913F8C715}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{EF88D0AD-6763-4C9E-A952-C649B59621B9}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{E20F8589-E704-472F-8210-F61763541890}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{9C05DDC5-8C71-475C-9F54-8EAEDF382E1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Chhanged the A link to a P ele for cleare UX
</commit_message>
<xml_diff>
--- a/ZorgTools.xlsx
+++ b/ZorgTools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\S5 Stage\InterActiveList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75887A7E-1246-4F68-8780-992BCB83BF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07989546-87CF-4DE2-AB1F-2101F4A2F70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E00BBEE8-4644-4DCA-8691-B52A139901BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>E-health:Beeldbellen, ECD Electronisch clienten dossier</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>https://Google.nl/,https://stackoverflow.com/questions/179713/how-to-change-the-href-attribute-for-a-hyperlink-using-jquery</t>
+  </si>
+  <si>
+    <t>https://github.com/justinvandelaar/InteractiveList</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,8 +544,8 @@
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -626,8 +629,9 @@
     <hyperlink ref="C5" r:id="rId4" xr:uid="{EF88D0AD-6763-4C9E-A952-C649B59621B9}"/>
     <hyperlink ref="D2" r:id="rId5" xr:uid="{E20F8589-E704-472F-8210-F61763541890}"/>
     <hyperlink ref="D3" r:id="rId6" xr:uid="{9C05DDC5-8C71-475C-9F54-8EAEDF382E1F}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{46C1D880-7D5D-4BF1-A194-4E128E89E08C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a few UI/UX changes and a Instruction manual
</commit_message>
<xml_diff>
--- a/ZorgTools.xlsx
+++ b/ZorgTools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\S5 Stage\InterActiveList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07989546-87CF-4DE2-AB1F-2101F4A2F70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9869EA33-4BE3-4CE7-8EF3-4C713C18E1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E00BBEE8-4644-4DCA-8691-B52A139901BC}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +133,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -480,7 +486,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,6 +628,7 @@
       <c r="B20" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{2E623B92-F184-4918-A35F-B63234A80043}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{B46671C8-63A3-49B5-B4EF-1CACFB8A9760}"/>

</xml_diff>